<commit_message>
tests implemented & mass/charge balance fixed
</commit_message>
<xml_diff>
--- a/pyexsimo/models/liver_glucose_annotations.xlsx
+++ b/pyexsimo/models/liver_glucose_annotations.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2613" uniqueCount="654">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2613" uniqueCount="655">
   <si>
     <t xml:space="preserve">pattern</t>
   </si>
@@ -58,35 +58,7 @@
     <t xml:space="preserve">non-spatial continuous framework</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">^[\w+,_]*glucose</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">[\w+,_]*</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">$</t>
-    </r>
+    <t xml:space="preserve">^[\w+,_]*glucose[\w+,_]*$</t>
   </si>
   <si>
     <t xml:space="preserve">model</t>
@@ -1889,6 +1861,9 @@
     <t xml:space="preserve">inchikey/DTBNBXWJWCWCIK-UHFFFAOYSA-K</t>
   </si>
   <si>
+    <t xml:space="preserve">C3H2O6P</t>
+  </si>
+  <si>
     <t xml:space="preserve">^pyr[_,\w]*$</t>
   </si>
   <si>
@@ -1904,7 +1879,7 @@
     <t xml:space="preserve">inchikey/LCTONWCANYUPML-UHFFFAOYSA-M</t>
   </si>
   <si>
-    <t xml:space="preserve">C3H2O6P</t>
+    <t xml:space="preserve">C3H3O3</t>
   </si>
   <si>
     <t xml:space="preserve">^oaa[_,\w]*$</t>
@@ -1922,7 +1897,7 @@
     <t xml:space="preserve">inchikey/KHPXUQMNIQBQEV-UHFFFAOYSA-L</t>
   </si>
   <si>
-    <t xml:space="preserve">C3H3O3</t>
+    <t xml:space="preserve">C4H2O5</t>
   </si>
   <si>
     <t xml:space="preserve">^lac[_,\w]*$</t>
@@ -1940,7 +1915,7 @@
     <t xml:space="preserve">inchikey/JVTAAEKCZFNVCJ-REOHCLBHSA-M</t>
   </si>
   <si>
-    <t xml:space="preserve">C4H2O5</t>
+    <t xml:space="preserve">C3H5O3</t>
   </si>
   <si>
     <t xml:space="preserve">^coa[_,\w]*$</t>
@@ -2020,7 +1995,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -2064,12 +2039,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -2254,8 +2223,8 @@
   </sheetPr>
   <dimension ref="A1:AMH566"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A114" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E123" activeCellId="0" sqref="E123"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A490" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E535" activeCellId="0" sqref="E535"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14307,7 +14276,7 @@
       </c>
       <c r="F519" s="8"/>
     </row>
-    <row r="520" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="520" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A520" s="7" t="s">
         <v>608</v>
       </c>
@@ -14319,7 +14288,7 @@
       </c>
       <c r="D520" s="5"/>
       <c r="E520" s="6" t="s">
-        <v>602</v>
+        <v>613</v>
       </c>
       <c r="F520" s="0"/>
     </row>
@@ -14349,7 +14318,7 @@
     </row>
     <row r="523" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A523" s="7" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="B523" s="5" t="s">
         <v>421</v>
@@ -14369,7 +14338,7 @@
     </row>
     <row r="524" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A524" s="7" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="B524" s="5" t="s">
         <v>421</v>
@@ -14381,13 +14350,13 @@
         <v>25</v>
       </c>
       <c r="E524" s="5" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="F524" s="0"/>
     </row>
     <row r="525" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A525" s="7" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="B525" s="5" t="s">
         <v>421</v>
@@ -14399,15 +14368,15 @@
         <v>17</v>
       </c>
       <c r="E525" s="5" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="F525" s="0" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
     </row>
     <row r="526" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A526" s="7" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="B526" s="5" t="s">
         <v>421</v>
@@ -14419,13 +14388,13 @@
         <v>17</v>
       </c>
       <c r="E526" s="5" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="F526" s="0"/>
     </row>
-    <row r="527" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="527" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A527" s="7" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="B527" s="5" t="s">
         <v>421</v>
@@ -14435,13 +14404,13 @@
       </c>
       <c r="D527" s="5"/>
       <c r="E527" s="6" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="F527" s="0"/>
     </row>
     <row r="528" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A528" s="7" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="B528" s="5" t="s">
         <v>421</v>
@@ -14451,7 +14420,7 @@
       </c>
       <c r="D528" s="5"/>
       <c r="E528" s="9" t="s">
-        <v>481</v>
+        <v>488</v>
       </c>
       <c r="F528" s="0"/>
     </row>
@@ -14465,7 +14434,7 @@
     </row>
     <row r="530" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A530" s="7" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="B530" s="5" t="s">
         <v>421</v>
@@ -14485,7 +14454,7 @@
     </row>
     <row r="531" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A531" s="7" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="B531" s="5" t="s">
         <v>421</v>
@@ -14497,13 +14466,13 @@
         <v>25</v>
       </c>
       <c r="E531" s="5" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="F531" s="0"/>
     </row>
     <row r="532" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A532" s="7" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="B532" s="5" t="s">
         <v>421</v>
@@ -14515,15 +14484,15 @@
         <v>17</v>
       </c>
       <c r="E532" s="5" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="F532" s="8" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
     </row>
     <row r="533" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A533" s="7" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="B533" s="5" t="s">
         <v>421</v>
@@ -14535,13 +14504,13 @@
         <v>17</v>
       </c>
       <c r="E533" s="5" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="F533" s="8"/>
     </row>
-    <row r="534" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="534" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A534" s="7" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="B534" s="5" t="s">
         <v>421</v>
@@ -14551,13 +14520,13 @@
       </c>
       <c r="D534" s="5"/>
       <c r="E534" s="6" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="F534" s="0"/>
     </row>
     <row r="535" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A535" s="7" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="B535" s="5" t="s">
         <v>421</v>
@@ -14567,7 +14536,7 @@
       </c>
       <c r="D535" s="5"/>
       <c r="E535" s="9" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="F535" s="0"/>
     </row>
@@ -14581,7 +14550,7 @@
     </row>
     <row r="537" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A537" s="7" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="B537" s="5" t="s">
         <v>421</v>
@@ -14601,7 +14570,7 @@
     </row>
     <row r="538" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A538" s="7" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="B538" s="5" t="s">
         <v>421</v>
@@ -14613,13 +14582,13 @@
         <v>25</v>
       </c>
       <c r="E538" s="5" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="F538" s="0"/>
     </row>
     <row r="539" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A539" s="7" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="B539" s="5" t="s">
         <v>421</v>
@@ -14631,15 +14600,15 @@
         <v>17</v>
       </c>
       <c r="E539" s="5" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="F539" s="8" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
     </row>
     <row r="540" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A540" s="7" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="B540" s="5" t="s">
         <v>421</v>
@@ -14651,13 +14620,13 @@
         <v>17</v>
       </c>
       <c r="E540" s="5" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="F540" s="8"/>
     </row>
-    <row r="541" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="541" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A541" s="7" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="B541" s="5" t="s">
         <v>421</v>
@@ -14667,13 +14636,13 @@
       </c>
       <c r="D541" s="0"/>
       <c r="E541" s="6" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="F541" s="0"/>
     </row>
     <row r="542" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A542" s="7" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="B542" s="5" t="s">
         <v>421</v>
@@ -14683,7 +14652,7 @@
       </c>
       <c r="D542" s="5"/>
       <c r="E542" s="9" t="s">
-        <v>495</v>
+        <v>488</v>
       </c>
       <c r="F542" s="0"/>
     </row>
@@ -14697,7 +14666,7 @@
     </row>
     <row r="544" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A544" s="7" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="B544" s="5" t="s">
         <v>421</v>
@@ -14717,7 +14686,7 @@
     </row>
     <row r="545" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A545" s="7" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="B545" s="5" t="s">
         <v>421</v>
@@ -14729,13 +14698,13 @@
         <v>25</v>
       </c>
       <c r="E545" s="5" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="F545" s="0"/>
     </row>
     <row r="546" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A546" s="7" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="B546" s="5" t="s">
         <v>421</v>
@@ -14747,15 +14716,15 @@
         <v>17</v>
       </c>
       <c r="E546" s="5" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="F546" s="8" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
     </row>
     <row r="547" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A547" s="7" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="B547" s="5" t="s">
         <v>421</v>
@@ -14767,13 +14736,13 @@
         <v>17</v>
       </c>
       <c r="E547" s="5" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="F547" s="8"/>
     </row>
     <row r="548" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A548" s="7" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="B548" s="5" t="s">
         <v>421</v>
@@ -14783,13 +14752,13 @@
       </c>
       <c r="D548" s="0"/>
       <c r="E548" s="6" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="F548" s="0"/>
     </row>
     <row r="549" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A549" s="7" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="B549" s="5" t="s">
         <v>421</v>
@@ -14813,7 +14782,7 @@
     </row>
     <row r="551" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A551" s="7" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="B551" s="5" t="s">
         <v>421</v>
@@ -14833,7 +14802,7 @@
     </row>
     <row r="552" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A552" s="7" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="B552" s="5" t="s">
         <v>421</v>
@@ -14845,13 +14814,13 @@
         <v>25</v>
       </c>
       <c r="E552" s="5" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="F552" s="0"/>
     </row>
     <row r="553" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A553" s="7" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="B553" s="5" t="s">
         <v>421</v>
@@ -14863,15 +14832,15 @@
         <v>17</v>
       </c>
       <c r="E553" s="5" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
       <c r="F553" s="8" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
     </row>
     <row r="554" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A554" s="7" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="B554" s="5" t="s">
         <v>421</v>
@@ -14883,13 +14852,13 @@
         <v>17</v>
       </c>
       <c r="E554" s="5" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="F554" s="8"/>
     </row>
     <row r="555" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A555" s="7" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="B555" s="5" t="s">
         <v>421</v>
@@ -14899,13 +14868,13 @@
       </c>
       <c r="D555" s="0"/>
       <c r="E555" s="6" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="F555" s="0"/>
     </row>
     <row r="556" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A556" s="7" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="B556" s="5" t="s">
         <v>421</v>
@@ -14929,7 +14898,7 @@
     </row>
     <row r="558" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A558" s="7" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="B558" s="5" t="s">
         <v>421</v>
@@ -14949,7 +14918,7 @@
     </row>
     <row r="559" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A559" s="7" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="B559" s="5" t="s">
         <v>421</v>
@@ -14961,13 +14930,13 @@
         <v>25</v>
       </c>
       <c r="E559" s="5" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="F559" s="0"/>
     </row>
     <row r="560" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A560" s="7" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="B560" s="5" t="s">
         <v>421</v>
@@ -14979,15 +14948,15 @@
         <v>17</v>
       </c>
       <c r="E560" s="5" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="F560" s="8" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
     </row>
     <row r="561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A561" s="7" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="B561" s="5" t="s">
         <v>421</v>
@@ -14999,13 +14968,13 @@
         <v>17</v>
       </c>
       <c r="E561" s="5" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="F561" s="8"/>
     </row>
     <row r="562" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A562" s="7" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="B562" s="5" t="s">
         <v>421</v>
@@ -15015,13 +14984,13 @@
       </c>
       <c r="D562" s="0"/>
       <c r="E562" s="6" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="F562" s="0"/>
     </row>
     <row r="563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A563" s="7" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="B563" s="5" t="s">
         <v>421</v>
@@ -15045,7 +15014,7 @@
     </row>
     <row r="565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A565" s="3" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="B565" s="4"/>
       <c r="C565" s="4"/>
@@ -15055,10 +15024,10 @@
     </row>
     <row r="566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A566" s="5" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="B566" s="5" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
       <c r="C566" s="5" t="s">
         <v>8</v>
@@ -15067,10 +15036,10 @@
         <v>17</v>
       </c>
       <c r="E566" s="5" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="F566" s="6" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
     </row>
   </sheetData>

</xml_diff>